<commit_message>
Modifed all APIs according to change in Course model
</commit_message>
<xml_diff>
--- a/data/teachers_info.xlsx
+++ b/data/teachers_info.xlsx
@@ -978,7 +978,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>سیدمصطفی سیادت موسوی</t>
+          <t>سید مصطفی سیادت موسوی</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1233,7 +1233,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>سیدمحمد شهرتاش</t>
+          <t>سید محمد شهرتاش</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1273,7 +1273,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>سیدمحمدرضا موسوی میرکلایی</t>
+          <t>سید محمدرضا موسوی میرکلایی</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2213,7 +2213,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>سیدحسن هاشم آبادی</t>
+          <t>سید حسن هاشم آبادی</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2228,7 +2228,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>سیدمحمد سیدحسینی</t>
+          <t>سید محمد</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -2473,7 +2473,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>سیدهاشم مسدد</t>
+          <t>سیده اشم مسدد</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -2518,7 +2518,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>سیدسعید سیادت نژاد</t>
+          <t>سید سعید سیادت نژاد</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -2938,7 +2938,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>سیداصغر موسوی</t>
+          <t>سید اصغر موسوی</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -3568,7 +3568,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>سیدسینا ثمره موسوی</t>
+          <t>سید سینا ثمره موسوی</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
@@ -3583,7 +3583,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>سیدمهدی عطیفه کمال ابادفراهان</t>
+          <t>سید مهدی عطیفه کمال ابادفراهان</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
@@ -4623,7 +4623,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>سیدسپهر موسوی</t>
+          <t>سید سپهر موسوی</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
@@ -4638,7 +4638,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>سیدعلی نیک نام</t>
+          <t>سید علی نیک نام</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
@@ -4838,7 +4838,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>سیدمهدی علوی املشی</t>
+          <t>سید مهدی علوی املشی</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -5008,7 +5008,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>سیدسجاد میرولد</t>
+          <t>سید سجاد میرولد</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -5868,7 +5868,7 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>سیدجواد امامی</t>
+          <t>سید جواد امامی</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
@@ -5913,7 +5913,7 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>سیدحسن صدیقی</t>
+          <t>سید حسن صدیقی</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
@@ -6413,7 +6413,7 @@
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>سیدصالح اعتمادی</t>
+          <t>سید صالح اعتمادی</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
@@ -6543,7 +6543,7 @@
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>سیدمجید هاشمیان زاده</t>
+          <t>سید مجید هاشمیان زاده</t>
         </is>
       </c>
       <c r="C394" t="inlineStr">
@@ -7298,7 +7298,7 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>سیدحجت سبزپوشان</t>
+          <t>سید حجت سبزپوشان</t>
         </is>
       </c>
       <c r="C443" t="inlineStr">
@@ -7548,7 +7548,7 @@
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>دکتر سید حسین حسینی شکوه</t>
+          <t>سید حسین حسینی شکوه</t>
         </is>
       </c>
       <c r="C459" t="inlineStr">
@@ -7763,7 +7763,7 @@
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>سیدمحمدمهدی عبیری</t>
+          <t>سید محمدمهدی عبیری</t>
         </is>
       </c>
       <c r="C473" t="inlineStr">
@@ -7993,7 +7993,7 @@
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>سیدمیعاد صالحی</t>
+          <t>سید میعاد صالحی</t>
         </is>
       </c>
       <c r="C488" t="inlineStr">
@@ -8333,7 +8333,7 @@
     <row r="510">
       <c r="A510" t="inlineStr">
         <is>
-          <t>سیدحسین سیدین</t>
+          <t>سید حسین</t>
         </is>
       </c>
       <c r="C510" t="inlineStr">
@@ -8603,7 +8603,7 @@
     <row r="528">
       <c r="A528" t="inlineStr">
         <is>
-          <t>سیدعبدالهادی دانشپور</t>
+          <t>سید عبدالهادی دانشپور</t>
         </is>
       </c>
       <c r="C528" t="inlineStr">
@@ -9758,7 +9758,7 @@
     <row r="603">
       <c r="A603" t="inlineStr">
         <is>
-          <t>محسن پور سیداقایی</t>
+          <t>سید اقایی</t>
         </is>
       </c>
       <c r="C603" t="inlineStr">
@@ -9788,7 +9788,7 @@
     <row r="605">
       <c r="A605" t="inlineStr">
         <is>
-          <t>سیدمصطفی حسینعلی پور</t>
+          <t>سید مصطفی حسینعلی پور</t>
         </is>
       </c>
       <c r="C605" t="inlineStr">
@@ -9963,7 +9963,7 @@
     <row r="616">
       <c r="A616" t="inlineStr">
         <is>
-          <t>سیدادریس فیض آبادی</t>
+          <t>سید ادریس فیض آبادی</t>
         </is>
       </c>
       <c r="C616" t="inlineStr">
@@ -10073,7 +10073,7 @@
     <row r="623">
       <c r="A623" t="inlineStr">
         <is>
-          <t>سیدمحمدعلی بوترابی</t>
+          <t>سید محمدعلی بوترابی</t>
         </is>
       </c>
       <c r="C623" t="inlineStr">
@@ -10853,7 +10853,7 @@
     <row r="675">
       <c r="A675" t="inlineStr">
         <is>
-          <t>سیدجواد ازهری</t>
+          <t>سید جواد ازهری</t>
         </is>
       </c>
       <c r="C675" t="inlineStr">
@@ -10868,7 +10868,7 @@
     <row r="676">
       <c r="A676" t="inlineStr">
         <is>
-          <t>سیدنظام الدین اشرفی زاده</t>
+          <t>سید نظام الدین اشرفی زاده</t>
         </is>
       </c>
       <c r="C676" t="inlineStr">
@@ -10948,7 +10948,7 @@
     <row r="681">
       <c r="A681" t="inlineStr">
         <is>
-          <t>سیدمحمدعلی موسوی</t>
+          <t>سید محمدعلی موسوی</t>
         </is>
       </c>
       <c r="C681" t="inlineStr">
@@ -11243,7 +11243,7 @@
     <row r="700">
       <c r="A700" t="inlineStr">
         <is>
-          <t>سیدذبیح الله طباطبایی شیرازانی</t>
+          <t>سید ذبیح الله طباطبایی شیرازانی</t>
         </is>
       </c>
       <c r="C700" t="inlineStr">
@@ -11558,7 +11558,7 @@
     <row r="721">
       <c r="A721" t="inlineStr">
         <is>
-          <t>سیدمحمود میرطباطبایی</t>
+          <t>سید محمود میرطباطبایی</t>
         </is>
       </c>
       <c r="C721" t="inlineStr">
@@ -12078,7 +12078,7 @@
     <row r="755">
       <c r="A755" t="inlineStr">
         <is>
-          <t>سیدمجید مفیدی شمیرانی</t>
+          <t>سید مجید مفیدی شمیرانی</t>
         </is>
       </c>
       <c r="C755" t="inlineStr">
@@ -13323,7 +13323,7 @@
     <row r="837">
       <c r="A837" t="inlineStr">
         <is>
-          <t>سیدمجتبی حسینی نسب</t>
+          <t>سید مجتبی حسینی نسب</t>
         </is>
       </c>
       <c r="C837" t="inlineStr">
@@ -13843,7 +13843,7 @@
     <row r="871">
       <c r="A871" t="inlineStr">
         <is>
-          <t>سیداصغر ابن الرسول</t>
+          <t>سید اصغر ابن الرسول</t>
         </is>
       </c>
       <c r="C871" t="inlineStr">
@@ -13948,7 +13948,7 @@
     <row r="878">
       <c r="A878" t="inlineStr">
         <is>
-          <t>سیدامیر منصوری</t>
+          <t>سید امیر منصوری</t>
         </is>
       </c>
       <c r="C878" t="inlineStr">
@@ -14528,7 +14528,7 @@
     <row r="916">
       <c r="A916" t="inlineStr">
         <is>
-          <t>سیدرضا علمی حسینی</t>
+          <t>سید رضا علمی حسینی</t>
         </is>
       </c>
       <c r="C916" t="inlineStr">
@@ -14543,7 +14543,7 @@
     <row r="917">
       <c r="A917" t="inlineStr">
         <is>
-          <t>سیدمجتبی میرحسینی</t>
+          <t>سید مجتبی میرحسینی</t>
         </is>
       </c>
       <c r="C917" t="inlineStr">
@@ -14768,7 +14768,7 @@
     <row r="932">
       <c r="A932" t="inlineStr">
         <is>
-          <t>سیدعلی حسینی</t>
+          <t>سید علی حسینی</t>
         </is>
       </c>
       <c r="C932" t="inlineStr">
@@ -15408,7 +15408,7 @@
     <row r="974">
       <c r="A974" t="inlineStr">
         <is>
-          <t>سیدمهدی حسینی دولت آبادی</t>
+          <t>سید مهدی حسینی دولت آبادی</t>
         </is>
       </c>
       <c r="C974" t="inlineStr">
@@ -15498,7 +15498,7 @@
     <row r="980">
       <c r="A980" t="inlineStr">
         <is>
-          <t>سیدعلی قهاری</t>
+          <t>سید علی قهاری</t>
         </is>
       </c>
       <c r="C980" t="inlineStr">
@@ -15578,7 +15578,7 @@
     <row r="985">
       <c r="A985" t="inlineStr">
         <is>
-          <t>سیدحسن موسوی</t>
+          <t>سید حسن موسوی</t>
         </is>
       </c>
       <c r="C985" t="inlineStr">
@@ -15623,7 +15623,7 @@
     <row r="988">
       <c r="A988" t="inlineStr">
         <is>
-          <t>سیدحامد رستگار</t>
+          <t>سید حامد رستگار</t>
         </is>
       </c>
       <c r="C988" t="inlineStr">
@@ -15913,7 +15913,7 @@
     <row r="1007">
       <c r="A1007" t="inlineStr">
         <is>
-          <t>سیدابوالفضل حسینی زاده</t>
+          <t>سید ابوالفضل حسینی زاده</t>
         </is>
       </c>
       <c r="C1007" t="inlineStr">
@@ -15988,7 +15988,7 @@
     <row r="1012">
       <c r="A1012" t="inlineStr">
         <is>
-          <t>سید علیرضا سیدوکیلی</t>
+          <t>سید علیرضا</t>
         </is>
       </c>
       <c r="B1012" t="inlineStr">
@@ -16263,7 +16263,7 @@
     <row r="1030">
       <c r="A1030" t="inlineStr">
         <is>
-          <t>سیددانیال غفاریان تربتی مجاور</t>
+          <t>سید دانیال غفاریان تربتی مجاور</t>
         </is>
       </c>
       <c r="C1030" t="inlineStr">
@@ -16368,7 +16368,7 @@
     <row r="1037">
       <c r="A1037" t="inlineStr">
         <is>
-          <t>سیدعلی سرکشیکیان</t>
+          <t>سید علی سرکشیکیان</t>
         </is>
       </c>
       <c r="C1037" t="inlineStr">
@@ -16863,7 +16863,7 @@
     <row r="1070">
       <c r="A1070" t="inlineStr">
         <is>
-          <t>سید حمید حاجی سیدجوادی</t>
+          <t>سید حمید حاجی</t>
         </is>
       </c>
       <c r="C1070" t="inlineStr">
@@ -17013,7 +17013,7 @@
     <row r="1080">
       <c r="A1080" t="inlineStr">
         <is>
-          <t>سیدحسن ذبیحی فر</t>
+          <t>سید حسن ذبیحی فر</t>
         </is>
       </c>
       <c r="C1080" t="inlineStr">

</xml_diff>